<commit_message>
terminado el doc de reqs
</commit_message>
<xml_diff>
--- a/Rqnf.xlsx
+++ b/Rqnf.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8640"/>
+    <workbookView windowWidth="20385" windowHeight="8640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
   <si>
     <t>clave</t>
   </si>
@@ -68,6 +69,141 @@
   </si>
   <si>
     <t>el sistema no debe realizar tranzaciones con otros sistemas</t>
+  </si>
+  <si>
+    <t>Requerimiento no funcional de Implementacion [RQNFI]</t>
+  </si>
+  <si>
+    <t>Clave</t>
+  </si>
+  <si>
+    <t>Requerimiento</t>
+  </si>
+  <si>
+    <t>RQNFI01</t>
+  </si>
+  <si>
+    <t>RQNFI02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el sistema debe iniciar  en maximo 5 segundos </t>
+  </si>
+  <si>
+    <t>RQNFI03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el sistema debe apagarse en maximo 5 segundos </t>
+  </si>
+  <si>
+    <t>RQNFI04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el registro de entrada de personal debe realizarse en maximo 5 segundos </t>
+  </si>
+  <si>
+    <t>RQNFI05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el registro de salida  del personal debe realizarse en maximo 5 segundos </t>
+  </si>
+  <si>
+    <t>RQNFI06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dl registro de entrada de cliente debe realizarse en maximo 5 segundos </t>
+  </si>
+  <si>
+    <t>RQNFI07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el registro de salida  del cliente debe realizarse en maximo 5 segundos </t>
+  </si>
+  <si>
+    <t>RQNFI08</t>
+  </si>
+  <si>
+    <t>RQNFI09</t>
+  </si>
+  <si>
+    <t>el sistema debe solicitar contraseñas para cumplir req anterior</t>
+  </si>
+  <si>
+    <t>RQNFI10</t>
+  </si>
+  <si>
+    <t>el sistema debe mostrar notificaciones mediante ventanas emergentes</t>
+  </si>
+  <si>
+    <t>RQNFI11</t>
+  </si>
+  <si>
+    <t>el sistema debe asegurar que sus notificaciones sean confiables(concuerden con las reglas de neocio)</t>
+  </si>
+  <si>
+    <t>RQNFI12</t>
+  </si>
+  <si>
+    <t>el sistema debe ser creado para sistemas operativos windows</t>
+  </si>
+  <si>
+    <t>RQNFI13</t>
+  </si>
+  <si>
+    <t>el sistema operativo minimo debe ser windows 7</t>
+  </si>
+  <si>
+    <t>RQNFI14</t>
+  </si>
+  <si>
+    <t>el sistema operativo debe tener instalado el framework .NET</t>
+  </si>
+  <si>
+    <t>RQNFI15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el sistema debe usar la version 3.5 del framework .NET o superiores </t>
+  </si>
+  <si>
+    <t>RQNFI16</t>
+  </si>
+  <si>
+    <t>RQNFI17</t>
+  </si>
+  <si>
+    <t>RQNFI18</t>
+  </si>
+  <si>
+    <t>RQNFI19</t>
+  </si>
+  <si>
+    <t>el sistema no debe realizar tranzaciones con otro hardware</t>
+  </si>
+  <si>
+    <t>Requerimiento no funcional de Registro [RQNFR]</t>
+  </si>
+  <si>
+    <t>RQNFR01</t>
+  </si>
+  <si>
+    <t>el sistema debe tener elementos de respuesta a fallos de lectura de codigo</t>
+  </si>
+  <si>
+    <t>RQNFR02</t>
+  </si>
+  <si>
+    <t>el sistema debe contar con un panel de registro manual ante fallos de lectura de codio QR</t>
+  </si>
+  <si>
+    <t>RQNFR03</t>
+  </si>
+  <si>
+    <t>el sistema debe registrar la entrada de los cliente mediante un lector de codigo QR</t>
+  </si>
+  <si>
+    <t>RQNFR04</t>
+  </si>
+  <si>
+    <t>el sistema debe leer y procesar un codio QR en MAXIMO 5 SEGUNDOS</t>
   </si>
 </sst>
 </file>
@@ -75,12 +211,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +225,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -104,16 +270,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -128,14 +301,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -143,45 +332,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,45 +384,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,187 +401,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,21 +644,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -508,13 +658,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,158 +687,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1004,7 +1181,7 @@
   <sheetPr/>
   <dimension ref="A3:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
@@ -1105,4 +1282,239 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="C2:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <cols>
+    <col min="4" max="4" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:4">
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="3:4">
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4">
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4">
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4">
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4">
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4">
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4">
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4">
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4">
+      <c r="C24" s="3"/>
+      <c r="D24" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4">
+      <c r="C25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4">
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4">
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4">
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4">
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>